<commit_message>
functions quiz-1 done successfully - 100 of 100
</commit_message>
<xml_diff>
--- a/8_CU_Program/3_Integrals/Integrals.xlsx
+++ b/8_CU_Program/3_Integrals/Integrals.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\8_CU_Program\3_Integrals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCB4DC6-085F-4211-BEDD-C6C327A59904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B323B18F-5C29-4F1E-BE63-0A3DE82327EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="calcs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,6 +101,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>472534</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30514</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691EA2CE-B755-0D3F-55EB-C8218827120F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="1463040"/>
+          <a:ext cx="1082134" cy="396274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:F6"/>
+  <dimension ref="C3:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,7 +478,20 @@
         <v>371.66666666666669</v>
       </c>
     </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <f>4*EXP(-2*-2)</f>
+        <v>218.39260013257694</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="e">
+        <f>SQRT(-10+6)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integration by parts assignment done on ipad
</commit_message>
<xml_diff>
--- a/8_CU_Program/3_Integrals/Integrals.xlsx
+++ b/8_CU_Program/3_Integrals/Integrals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\8_CU_Program\3_Integrals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F6EAF3-5556-41AD-8224-89C84D433591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AEE7A1-399F-4DF5-B70A-FC2F2F049376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,19 +36,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>x3/3</t>
   </si>
   <si>
     <t>10x</t>
   </si>
+  <si>
+    <t>4*e^(-2*t)</t>
+  </si>
+  <si>
+    <t>e^2*(1)</t>
+  </si>
+  <si>
+    <t>e^0*(-1)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +68,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
@@ -83,9 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:H15"/>
+  <dimension ref="C3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,6 +511,9 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="G12" s="1">
         <f>2/3</f>
         <v>0.66666666666666663</v>
@@ -511,9 +530,31 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="1" t="e">
-        <f>SQRT(-10+6)</f>
-        <v>#NUM!</v>
+      <c r="C15" s="1">
+        <f>SQRT(10+6)</f>
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="1">
+        <f>EXP(2)</f>
+        <v>7.3890560989306504</v>
+      </c>
+      <c r="H16" s="1">
+        <f>EXP(0)*(-1)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="1">
+        <f>G16-H16</f>
+        <v>8.3890560989306504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>